<commit_message>
Se refactorizaron todas las clases para obtener en los metodos y clases menos complejidad posible, se cambiaron todas las palabras al ingles para manejarlo en un solo idioma
</commit_message>
<xml_diff>
--- a/dias_de_sol.xlsx
+++ b/dias_de_sol.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Booking\Booking\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>Nombre</t>
   </si>
@@ -77,12 +77,37 @@
   </si>
   <si>
     <t>Bogota</t>
+  </si>
+  <si>
+    <t>Día Relax</t>
+  </si>
+  <si>
+    <t>120.0</t>
+  </si>
+  <si>
+    <t>Cartagena</t>
+  </si>
+  <si>
+    <t>Piscina, Spa, Yoga</t>
+  </si>
+  <si>
+    <t>150.0</t>
+  </si>
+  <si>
+    <t>Medellín</t>
+  </si>
+  <si>
+    <t>Senderismo, Rappel, Kayak</t>
+  </si>
+  <si>
+    <t>Bogotá</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -437,94 +462,163 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s" s="0">
         <v>10</v>
       </c>
     </row>

</xml_diff>